<commit_message>
clean data for Gloria
</commit_message>
<xml_diff>
--- a/Data/Summary_stats_all.xlsx
+++ b/Data/Summary_stats_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1aac\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2600" documentId="8_{93AF461B-AE72-4C0A-9557-C7A1114A39DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4705EF68-8B9D-4984-9B98-C637CCCB1226}"/>
+  <xr:revisionPtr revIDLastSave="2602" documentId="8_{93AF461B-AE72-4C0A-9557-C7A1114A39DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D4D81F73-B49D-4B85-A8C8-83160B23CCC2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="985" uniqueCount="369">
   <si>
     <t>location_name</t>
   </si>
@@ -180,7 +180,7 @@
     <t>bars_25</t>
   </si>
   <si>
-    <t>bar_33</t>
+    <t>bars_33</t>
   </si>
   <si>
     <t>bars_50</t>
@@ -273,7 +273,7 @@
     <t xml:space="preserve">gathering_limit </t>
   </si>
   <si>
-    <t>religious_gatherings</t>
+    <t>religious_gathering</t>
   </si>
   <si>
     <t>religious_limit_capacity</t>
@@ -867,9 +867,6 @@
     <t>Bars can open with 25% capacity</t>
   </si>
   <si>
-    <t>bars_33</t>
-  </si>
-  <si>
     <t>Bars can open with 33% capacity</t>
   </si>
   <si>
@@ -970,9 +967,6 @@
   </si>
   <si>
     <t>End of most extreme gathering restrictions</t>
-  </si>
-  <si>
-    <t>religious_gathering</t>
   </si>
   <si>
     <t>Most extreme restrictions for religous gatherings</t>
@@ -2046,8 +2040,8 @@
   <dimension ref="A1:CM52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CC2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="CH2" sqref="CH2"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BY2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="CB2" sqref="CB2"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -6553,8 +6547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1751FEF-4AD6-4594-B26C-014EFAF552D2}">
   <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6953,10 +6947,10 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" t="s">
         <v>277</v>
-      </c>
-      <c r="B40" t="s">
-        <v>278</v>
       </c>
       <c r="C40" t="s">
         <v>252</v>
@@ -6967,7 +6961,7 @@
         <v>49</v>
       </c>
       <c r="B41" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C41" t="s">
         <v>252</v>
@@ -6978,7 +6972,7 @@
         <v>50</v>
       </c>
       <c r="B42" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C42" t="s">
         <v>252</v>
@@ -6989,7 +6983,7 @@
         <v>51</v>
       </c>
       <c r="B43" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C43" t="s">
         <v>252</v>
@@ -7000,7 +6994,7 @@
         <v>52</v>
       </c>
       <c r="B44" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C44" t="s">
         <v>252</v>
@@ -7011,7 +7005,7 @@
         <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C45" t="s">
         <v>252</v>
@@ -7023,7 +7017,7 @@
         <v>54</v>
       </c>
       <c r="B46" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C46" t="s">
         <v>252</v>
@@ -7034,7 +7028,7 @@
         <v>55</v>
       </c>
       <c r="B47" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C47" t="s">
         <v>252</v>
@@ -7045,7 +7039,7 @@
         <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C48" t="s">
         <v>252</v>
@@ -7056,7 +7050,7 @@
         <v>57</v>
       </c>
       <c r="B49" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C49" t="s">
         <v>252</v>
@@ -7067,7 +7061,7 @@
         <v>58</v>
       </c>
       <c r="B50" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C50" t="s">
         <v>252</v>
@@ -7078,7 +7072,7 @@
         <v>59</v>
       </c>
       <c r="B51" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C51" t="s">
         <v>252</v>
@@ -7089,7 +7083,7 @@
         <v>60</v>
       </c>
       <c r="B52" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C52" t="s">
         <v>252</v>
@@ -7100,7 +7094,7 @@
         <v>61</v>
       </c>
       <c r="B53" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C53" t="s">
         <v>252</v>
@@ -7111,7 +7105,7 @@
         <v>62</v>
       </c>
       <c r="B54" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C54" t="s">
         <v>252</v>
@@ -7122,7 +7116,7 @@
         <v>63</v>
       </c>
       <c r="B55" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C55" t="s">
         <v>252</v>
@@ -7133,7 +7127,7 @@
         <v>64</v>
       </c>
       <c r="B56" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C56" t="s">
         <v>252</v>
@@ -7144,7 +7138,7 @@
         <v>65</v>
       </c>
       <c r="B57" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C57" t="s">
         <v>252</v>
@@ -7155,7 +7149,7 @@
         <v>66</v>
       </c>
       <c r="B58" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C58" t="s">
         <v>252</v>
@@ -7163,10 +7157,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="B59" t="s">
         <v>297</v>
-      </c>
-      <c r="B59" t="s">
-        <v>298</v>
       </c>
       <c r="C59" t="s">
         <v>252</v>
@@ -7177,7 +7171,7 @@
         <v>70</v>
       </c>
       <c r="B60" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C60" t="s">
         <v>252</v>
@@ -7188,7 +7182,7 @@
         <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C61" t="s">
         <v>252</v>
@@ -7199,7 +7193,7 @@
         <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C62" t="s">
         <v>252</v>
@@ -7210,7 +7204,7 @@
         <v>71</v>
       </c>
       <c r="B63" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C63" t="s">
         <v>252</v>
@@ -7221,7 +7215,7 @@
         <v>72</v>
       </c>
       <c r="B64" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C64" t="s">
         <v>252</v>
@@ -7232,7 +7226,7 @@
         <v>73</v>
       </c>
       <c r="B65" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C65" t="s">
         <v>252</v>
@@ -7243,10 +7237,10 @@
         <v>74</v>
       </c>
       <c r="B66" t="s">
+        <v>304</v>
+      </c>
+      <c r="C66" t="s">
         <v>305</v>
-      </c>
-      <c r="C66" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -7254,10 +7248,10 @@
         <v>75</v>
       </c>
       <c r="B67" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C67" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -7265,7 +7259,7 @@
         <v>77</v>
       </c>
       <c r="B68" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C68" t="s">
         <v>263</v>
@@ -7273,10 +7267,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="B69" t="s">
         <v>309</v>
-      </c>
-      <c r="B69" t="s">
-        <v>310</v>
       </c>
       <c r="C69" t="s">
         <v>263</v>
@@ -7287,7 +7281,7 @@
         <v>81</v>
       </c>
       <c r="B70" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C70" t="s">
         <v>263</v>
@@ -7295,10 +7289,10 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="11" t="s">
-        <v>312</v>
+        <v>79</v>
       </c>
       <c r="B71" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C71" t="s">
         <v>263</v>
@@ -7309,7 +7303,7 @@
         <v>80</v>
       </c>
       <c r="B72" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C72" t="s">
         <v>263</v>
@@ -7320,7 +7314,7 @@
         <v>82</v>
       </c>
       <c r="B73" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C73" t="s">
         <v>252</v>
@@ -7331,7 +7325,7 @@
         <v>83</v>
       </c>
       <c r="B74" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C74" t="s">
         <v>252</v>
@@ -7342,7 +7336,7 @@
         <v>84</v>
       </c>
       <c r="B75" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C75" t="s">
         <v>252</v>
@@ -7353,7 +7347,7 @@
         <v>85</v>
       </c>
       <c r="B76" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C76" t="s">
         <v>252</v>
@@ -7364,7 +7358,7 @@
         <v>86</v>
       </c>
       <c r="B77" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C77" t="s">
         <v>252</v>
@@ -7375,7 +7369,7 @@
         <v>87</v>
       </c>
       <c r="B78" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C78" t="s">
         <v>252</v>
@@ -7386,7 +7380,7 @@
         <v>88</v>
       </c>
       <c r="B79" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C79" t="s">
         <v>252</v>
@@ -7397,7 +7391,7 @@
         <v>89</v>
       </c>
       <c r="B80" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C80" t="s">
         <v>252</v>
@@ -7408,7 +7402,7 @@
         <v>19</v>
       </c>
       <c r="B81" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C81" t="s">
         <v>263</v>
@@ -7419,7 +7413,7 @@
         <v>20</v>
       </c>
       <c r="B82" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C82" t="s">
         <v>263</v>
@@ -7430,7 +7424,7 @@
         <v>21</v>
       </c>
       <c r="B83" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C83" t="s">
         <v>263</v>
@@ -7441,7 +7435,7 @@
         <v>15</v>
       </c>
       <c r="B84" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C84" t="s">
         <v>263</v>
@@ -7452,7 +7446,7 @@
         <v>16</v>
       </c>
       <c r="B85" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C85" t="s">
         <v>263</v>
@@ -7463,7 +7457,7 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C86" t="s">
         <v>263</v>
@@ -7474,7 +7468,7 @@
         <v>18</v>
       </c>
       <c r="B87" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C87" t="s">
         <v>263</v>
@@ -7485,7 +7479,7 @@
         <v>22</v>
       </c>
       <c r="B88" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C88" t="s">
         <v>263</v>
@@ -7496,7 +7490,7 @@
         <v>23</v>
       </c>
       <c r="B89" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C89" t="s">
         <v>263</v>
@@ -7525,76 +7519,76 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -7661,13 +7655,13 @@
         <v>33</v>
       </c>
       <c r="H1" t="s">
+        <v>348</v>
+      </c>
+      <c r="I1" t="s">
+        <v>349</v>
+      </c>
+      <c r="J1" t="s">
         <v>350</v>
-      </c>
-      <c r="I1" t="s">
-        <v>351</v>
-      </c>
-      <c r="J1" t="s">
-        <v>352</v>
       </c>
       <c r="K1" t="s">
         <v>47</v>
@@ -7718,10 +7712,10 @@
         <v>67</v>
       </c>
       <c r="AA1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="AB1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="AC1" t="s">
         <v>71</v>
@@ -7748,13 +7742,13 @@
         <v>83</v>
       </c>
       <c r="AK1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>354</v>
+      </c>
+      <c r="AM1" t="s">
         <v>355</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>356</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:39">
@@ -7762,7 +7756,7 @@
         <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C2" s="1">
         <v>43962</v>
@@ -7819,7 +7813,7 @@
         <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C3" s="1">
         <v>43959</v>
@@ -7831,7 +7825,7 @@
         <v>43959</v>
       </c>
       <c r="F3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G3" s="1">
         <v>43945</v>
@@ -7843,13 +7837,13 @@
         <v>43959</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="K3" s="1">
         <v>43959</v>
       </c>
       <c r="M3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="O3" s="1">
         <v>43945</v>
@@ -7859,13 +7853,13 @@
         <v>43959</v>
       </c>
       <c r="R3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="T3" s="1">
         <v>43959</v>
       </c>
       <c r="V3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="X3" s="1">
         <v>43945</v>
@@ -7906,7 +7900,7 @@
         <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C4" s="1">
         <v>43959</v>
@@ -7944,7 +7938,7 @@
         <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I5" s="13">
         <v>43960</v>
@@ -7970,7 +7964,7 @@
         <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="AC6" s="1">
         <v>43909</v>
@@ -7993,7 +7987,7 @@
         <v>107</v>
       </c>
       <c r="B7" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C7" s="1">
         <v>43952</v>
@@ -8031,7 +8025,7 @@
         <v>108</v>
       </c>
       <c r="B8" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C8" s="13">
         <v>43967</v>
@@ -8060,19 +8054,19 @@
         <v>109</v>
       </c>
       <c r="B9" t="s">
+        <v>356</v>
+      </c>
+      <c r="H9" t="s">
         <v>358</v>
       </c>
-      <c r="H9" t="s">
-        <v>360</v>
-      </c>
       <c r="I9" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="N9" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="W9" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="Z9" s="1">
         <v>43955</v>
@@ -8098,7 +8092,7 @@
         <v>110</v>
       </c>
       <c r="B10" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D10" s="1">
         <v>43962</v>
@@ -8137,7 +8131,7 @@
         <v>111</v>
       </c>
       <c r="B11" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="AC11" s="1">
         <v>43924</v>
@@ -8160,7 +8154,7 @@
         <v>117</v>
       </c>
       <c r="B12" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C12" s="13">
         <v>43955</v>
@@ -8189,7 +8183,7 @@
         <v>118</v>
       </c>
       <c r="B13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G13" s="1">
         <v>43967</v>
@@ -8233,16 +8227,16 @@
         <v>119</v>
       </c>
       <c r="B14" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C14" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D14" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G14" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="AC14" s="1">
         <v>43911</v>
@@ -8268,13 +8262,13 @@
         <v>122</v>
       </c>
       <c r="B15" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G15" s="1">
         <v>43955</v>
       </c>
       <c r="H15" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="L15" s="1">
         <v>43962</v>
@@ -8312,7 +8306,7 @@
         <v>125</v>
       </c>
       <c r="B16" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C16" s="1">
         <v>43959</v>
@@ -8356,7 +8350,7 @@
         <v>130</v>
       </c>
       <c r="B17" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C17" s="1">
         <v>43955</v>
@@ -8391,7 +8385,7 @@
         <v>134</v>
       </c>
       <c r="B18" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C18" s="1">
         <v>43971</v>
@@ -8403,10 +8397,10 @@
         <v>43973</v>
       </c>
       <c r="I18" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="N18" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="O18" s="1">
         <v>43973</v>
@@ -8435,7 +8429,7 @@
         <v>136</v>
       </c>
       <c r="B19" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D19" s="1">
         <v>43966</v>
@@ -8485,10 +8479,10 @@
         <v>139</v>
       </c>
       <c r="B20" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C20" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G20" s="1">
         <v>43952</v>
@@ -8497,16 +8491,16 @@
         <v>43952</v>
       </c>
       <c r="I20" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="N20" t="s">
+        <v>357</v>
+      </c>
+      <c r="S20" t="s">
         <v>359</v>
       </c>
-      <c r="S20" t="s">
-        <v>361</v>
-      </c>
       <c r="W20" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="X20" s="1">
         <v>43952</v>
@@ -8535,7 +8529,7 @@
         <v>142</v>
       </c>
       <c r="B21" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C21" s="1">
         <v>43966</v>
@@ -8565,25 +8559,25 @@
         <v>146</v>
       </c>
       <c r="B22" t="s">
+        <v>360</v>
+      </c>
+      <c r="C22" t="s">
+        <v>359</v>
+      </c>
+      <c r="G22" t="s">
         <v>362</v>
-      </c>
-      <c r="C22" t="s">
-        <v>361</v>
-      </c>
-      <c r="G22" t="s">
-        <v>364</v>
       </c>
       <c r="H22" s="1">
         <v>43962</v>
       </c>
       <c r="N22" t="s">
+        <v>357</v>
+      </c>
+      <c r="S22" t="s">
         <v>359</v>
       </c>
-      <c r="S22" t="s">
-        <v>361</v>
-      </c>
       <c r="W22" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="X22" s="1">
         <v>43976</v>
@@ -8609,19 +8603,19 @@
         <v>149</v>
       </c>
       <c r="B23" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C23" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="N23" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="S23" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="X23" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="AC23" s="1">
         <v>43914</v>
@@ -8647,7 +8641,7 @@
         <v>156</v>
       </c>
       <c r="B24" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C24" s="1">
         <v>43969</v>
@@ -8670,7 +8664,7 @@
         <v>159</v>
       </c>
       <c r="B25" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="AC25" s="1">
         <v>43924</v>
@@ -8699,7 +8693,7 @@
         <v>160</v>
       </c>
       <c r="B26" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C26" s="1">
         <v>43955</v>
@@ -8737,7 +8731,7 @@
         <v>162</v>
       </c>
       <c r="B27" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C27" s="1">
         <v>43948</v>
@@ -8746,7 +8740,7 @@
         <v>43947</v>
       </c>
       <c r="I27" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="N27" s="1">
         <v>43955</v>
@@ -8755,7 +8749,7 @@
         <v>43955</v>
       </c>
       <c r="W27" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="X27" s="1">
         <v>43947</v>
@@ -8790,7 +8784,7 @@
         <v>164</v>
       </c>
       <c r="B28" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="AE28" s="1">
         <v>43923</v>
@@ -8807,7 +8801,7 @@
         <v>167</v>
       </c>
       <c r="B29" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C29" s="1">
         <v>43960</v>
@@ -8848,7 +8842,7 @@
         <v>170</v>
       </c>
       <c r="B30" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C30" s="1">
         <v>43962</v>
@@ -8889,10 +8883,10 @@
         <v>172</v>
       </c>
       <c r="B31" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C31" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="Z31" s="1">
         <v>43969</v>
@@ -8921,28 +8915,28 @@
         <v>175</v>
       </c>
       <c r="B32" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C32" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G32" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="I32" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="L32" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="N32" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="Q32" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="W32" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="X32" s="1">
         <v>43952</v>
@@ -8971,28 +8965,28 @@
         <v>179</v>
       </c>
       <c r="B33" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C33" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G33" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="N33" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="S33" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="W33" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="X33" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="Z33" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="AC33" s="1">
         <v>43912</v>
@@ -9015,7 +9009,7 @@
         <v>182</v>
       </c>
       <c r="B34" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C34" s="1">
         <v>43959</v>
@@ -9053,7 +9047,7 @@
         <v>184</v>
       </c>
       <c r="B35" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C35" s="1">
         <v>43952</v>
@@ -9083,7 +9077,7 @@
         <v>186</v>
       </c>
       <c r="B36" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="O36" s="1">
         <v>43966</v>
@@ -9125,7 +9119,7 @@
         <v>189</v>
       </c>
       <c r="B37" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="I37" s="1">
         <v>43966</v>
@@ -9166,7 +9160,7 @@
         <v>192</v>
       </c>
       <c r="B38" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C38" s="1">
         <v>43966</v>
@@ -9178,10 +9172,10 @@
         <v>43966</v>
       </c>
       <c r="I38" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="J38" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="S38" s="1">
         <v>43966</v>
@@ -9216,34 +9210,34 @@
         <v>194</v>
       </c>
       <c r="B39" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C39" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G39" t="s">
+        <v>357</v>
+      </c>
+      <c r="H39" t="s">
         <v>359</v>
       </c>
-      <c r="H39" t="s">
-        <v>361</v>
-      </c>
       <c r="I39" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="J39" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="N39" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="O39" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="S39" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="W39" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="AC39" s="1">
         <v>43922</v>
@@ -9272,7 +9266,7 @@
         <v>196</v>
       </c>
       <c r="B40" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C40" s="1">
         <v>43969</v>
@@ -9311,7 +9305,7 @@
         <v>198</v>
       </c>
       <c r="B41" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C41" s="1">
         <v>43969</v>
@@ -9346,7 +9340,7 @@
         <v>201</v>
       </c>
       <c r="B42" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="Z42" s="1">
         <v>43949</v>
@@ -9366,7 +9360,7 @@
         <v>203</v>
       </c>
       <c r="B43" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="AC43" s="1">
         <v>43923</v>
@@ -9395,7 +9389,7 @@
         <v>205</v>
       </c>
       <c r="B44" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C44" s="1">
         <v>43955</v>
@@ -9433,7 +9427,7 @@
         <v>207</v>
       </c>
       <c r="B45" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="AE45" s="1">
         <v>43906</v>
@@ -9450,7 +9444,7 @@
         <v>209</v>
       </c>
       <c r="B46" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="AC46" s="1">
         <v>43914</v>
@@ -9496,31 +9490,31 @@
         <v>215</v>
       </c>
       <c r="C48" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G48" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="H48" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="I48" t="s">
+        <v>357</v>
+      </c>
+      <c r="J48" t="s">
+        <v>363</v>
+      </c>
+      <c r="K48" t="s">
+        <v>357</v>
+      </c>
+      <c r="Q48" t="s">
         <v>359</v>
       </c>
-      <c r="J48" t="s">
-        <v>365</v>
-      </c>
-      <c r="K48" t="s">
-        <v>359</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>361</v>
-      </c>
       <c r="R48" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="W48" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="X48" s="1">
         <v>43956</v>
@@ -9529,7 +9523,7 @@
         <v>191</v>
       </c>
       <c r="Z48" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="AC48" s="1">
         <v>43913</v>
@@ -9567,7 +9561,7 @@
         <v>43962</v>
       </c>
       <c r="Y49" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="Z49" s="1">
         <v>43951</v>
@@ -9661,7 +9655,7 @@
         <v>235</v>
       </c>
       <c r="C1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D1" t="s">
         <v>234</v>
@@ -9928,21 +9922,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BDEF0524A8DCAC4390DF2A201DBA1B23" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e26becf438bf4314338867ffb4daeb92">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="46584177-f7e1-4294-8a18-e9bbf41b5dbb" xmlns:ns3="e0881b95-ccce-4318-b214-db737a4c0e6d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7ad9550bc1a9b9d1f6cd6be240f61f96" ns2:_="" ns3:_="">
     <xsd:import namespace="46584177-f7e1-4294-8a18-e9bbf41b5dbb"/>
@@ -10147,8 +10126,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFA468C9-0F70-41CE-B16B-6BB10F131E16}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{518A3416-3BEE-4480-84C5-BE7DBA13BDBB}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10156,5 +10150,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{518A3416-3BEE-4480-84C5-BE7DBA13BDBB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFA468C9-0F70-41CE-B16B-6BB10F131E16}"/>
 </file>
</xml_diff>